<commit_message>
Results with IE256 phrase version
</commit_message>
<xml_diff>
--- a/data/combined.xlsx
+++ b/data/combined.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Word" sheetId="14" r:id="rId1"/>
@@ -11031,7 +11031,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A40:XFD44">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -44416,7 +44416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -46912,7 +46912,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B28:J44">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46924,8 +46924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47094,67 +47094,67 @@
         <v>4.5364166666699998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>868</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>0.34093333333300002</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>0.26928208333300002</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>0.26494875000000001</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>0.121734583333</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <v>0.10226125</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>9.9279583333300003E-2</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <v>0.12582083333300001</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="2">
         <v>9.3974166666699999E-2</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="2">
         <v>7.1522500000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>0.360063333333</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>0.27888291666699999</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>0.27666499999999999</v>
       </c>
       <c r="E7" s="2">
         <v>0.130415</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>0.105507083333</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>0.1038925</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>0.142139583333</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="2">
         <v>9.8862500000000006E-2</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="2">
         <v>7.7787499999999996E-2</v>
       </c>
     </row>
@@ -49199,7 +49199,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B28:J32">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49212,7 +49212,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A9"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54678,7 +54678,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A28:XFD32">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>